<commit_message>
:) I lost my sanity
</commit_message>
<xml_diff>
--- a/Assignment_6/DiffAssignmentL1.xlsx
+++ b/Assignment_6/DiffAssignmentL1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbold\Desktop\GNSS\Assignment_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBF74B-4BFE-4C6A-A4F3-6BD77330556E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55D8EDA-8927-497C-B88E-68562975572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="13">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="171" formatCode="0.000000000"/>
+    <numFmt numFmtId="172" formatCode="0.0000000000"/>
+    <numFmt numFmtId="174" formatCode="0.00000000000"/>
+    <numFmt numFmtId="175" formatCode="0.000000000000"/>
+    <numFmt numFmtId="176" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="177" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="178" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="185" formatCode="0.000000000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -206,7 +217,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,12 +329,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="185" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -965,16 +998,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1010,10 +1045,10 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="36">
         <v>23539463.375</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="36">
         <v>1655955.588</v>
       </c>
     </row>
@@ -1021,25 +1056,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="36">
         <v>23490620.344000001</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="36">
         <v>823151.02099999995</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="36">
         <v>21759846.219000001</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="36">
         <v>1790394.946</v>
       </c>
     </row>
@@ -1047,25 +1082,25 @@
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="36">
         <v>21711251.640999999</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="36">
         <v>896009.12100000004</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="36">
         <v>21465916.188000001</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="36">
         <v>-2239193.3280000002</v>
       </c>
     </row>
@@ -1073,25 +1108,25 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="36">
         <v>21416660.203000002</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="36">
         <v>-984361.76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="36">
         <v>20250933.188000001</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="36">
         <v>-104773.368</v>
       </c>
     </row>
@@ -1099,25 +1134,25 @@
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="36">
         <v>20201862.078000002</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="36">
         <v>12789.109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="36">
         <v>21883884.655999999</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="36">
         <v>-132527.399</v>
       </c>
     </row>
@@ -1125,25 +1160,25 @@
       <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="36">
         <v>21835232.258000001</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="36">
         <v>-3418.4389999999999</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="36">
         <v>22080151.719000001</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="36">
         <v>-1897452.8540000001</v>
       </c>
     </row>
@@ -1151,10 +1186,10 @@
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="36">
         <v>22030470.546999998</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="36">
         <v>-704176.24399999995</v>
       </c>
     </row>
@@ -1163,7 +1198,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="18">
+      <c r="C24" s="37">
         <v>-4.6269462519999999E-4</v>
       </c>
     </row>
@@ -1172,7 +1207,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="18">
+      <c r="C25" s="37">
         <v>-2.9888030410000002E-4</v>
       </c>
     </row>
@@ -1190,7 +1225,7 @@
       <c r="A28" s="16">
         <v>4</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="27">
         <v>448.59629794210201</v>
       </c>
     </row>
@@ -1198,7 +1233,7 @@
       <c r="A29" s="16">
         <v>5</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="26">
         <v>479.29772413521999</v>
       </c>
     </row>
@@ -1206,7 +1241,7 @@
       <c r="A30" s="16">
         <v>6</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="26">
         <v>-446.26960337162001</v>
       </c>
     </row>
@@ -1214,7 +1249,7 @@
       <c r="A31" s="16">
         <v>20</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="28">
         <v>54.324880238622399</v>
       </c>
     </row>
@@ -1222,7 +1257,7 @@
       <c r="A32" s="16">
         <v>24</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="28">
         <v>50.541296388953903</v>
       </c>
     </row>
@@ -1230,7 +1265,7 @@
       <c r="A33" s="16">
         <v>25</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="27">
         <v>-372.57383386418201</v>
       </c>
     </row>
@@ -1254,13 +1289,13 @@
         <v>13</v>
       </c>
       <c r="B37" s="14"/>
-      <c r="C37" s="16">
+      <c r="C37" s="21">
         <v>3099255.4493</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="18">
         <v>1014087.319</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="21">
         <v>5463148.7221999997</v>
       </c>
     </row>
@@ -1269,13 +1304,13 @@
         <v>34</v>
       </c>
       <c r="B38" s="14"/>
-      <c r="C38" s="16">
+      <c r="C38" s="21">
         <v>3099279.7204999998</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="21">
         <v>1013349.0864</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="21">
         <v>5463275.8063000003</v>
       </c>
     </row>
@@ -1304,92 +1339,92 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16">
+      <c r="A43" s="31">
         <v>4</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16">
+      <c r="B43" s="31"/>
+      <c r="C43" s="32">
         <v>-9640637.2448591292</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="33">
         <v>11963653.420836199</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E43" s="34">
         <v>21764864.538586002</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
+      <c r="A44" s="31">
         <v>5</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16">
+      <c r="B44" s="31"/>
+      <c r="C44" s="33">
         <v>11580980.2843192</v>
       </c>
-      <c r="D44" s="16">
+      <c r="D44" s="33">
         <v>18202692.292516202</v>
       </c>
-      <c r="E44" s="16">
+      <c r="E44" s="33">
         <v>15492885.826446399</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
+      <c r="A45" s="31">
         <v>6</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16">
+      <c r="B45" s="31"/>
+      <c r="C45" s="33">
         <v>22299882.173245899</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="35">
         <v>-922322.52783503395</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="33">
         <v>14645540.936491599</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="16">
+      <c r="A46" s="31">
         <v>20</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16">
+      <c r="B46" s="31"/>
+      <c r="C46" s="33">
         <v>15014113.589193899</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="32">
         <v>5240279.54006969</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E46" s="33">
         <v>21124797.4297668</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
+      <c r="A47" s="31">
         <v>24</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16">
+      <c r="B47" s="31"/>
+      <c r="C47" s="32">
         <v>2808519.2060025502</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D47" s="33">
         <v>17209982.446679398</v>
       </c>
-      <c r="E47" s="16">
+      <c r="E47" s="34">
         <v>20223860.699806999</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
+      <c r="A48" s="31">
         <v>25</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16">
+      <c r="B48" s="31"/>
+      <c r="C48" s="33">
         <v>8650991.1836913992</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D48" s="33">
         <v>-12956546.126773201</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="33">
         <v>21442358.524250198</v>
       </c>
     </row>
@@ -1402,19 +1437,19 @@
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="16">
+      <c r="A52" s="24">
         <v>104166.66666666701</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="E52" s="16">
+      <c r="E52" s="25">
         <v>-20833.333333333299</v>
       </c>
       <c r="F52">
@@ -1434,19 +1469,19 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
+      <c r="A53" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="24">
         <v>104166.66666666701</v>
       </c>
-      <c r="C53" s="16">
+      <c r="C53" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D53" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="E53" s="16">
+      <c r="E53" s="25">
         <v>-20833.333333333299</v>
       </c>
       <c r="F53">
@@ -1466,19 +1501,19 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="16">
+      <c r="A54" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="B54" s="16">
+      <c r="B54" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="C54" s="16">
+      <c r="C54" s="25">
         <v>104166.66666666701</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="E54" s="16">
+      <c r="E54" s="25">
         <v>-20833.333333333299</v>
       </c>
       <c r="F54">
@@ -1498,19 +1533,19 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
+      <c r="A55" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="B55" s="16">
+      <c r="B55" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C55" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="24">
         <v>104166.66666666701</v>
       </c>
-      <c r="E55" s="16">
+      <c r="E55" s="25">
         <v>-20833.333333333299</v>
       </c>
       <c r="F55">
@@ -1530,19 +1565,19 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
+      <c r="A56" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="B56" s="16">
+      <c r="B56" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="C56" s="16">
+      <c r="C56" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="25">
         <v>-20833.333333333299</v>
       </c>
-      <c r="E56" s="16">
+      <c r="E56" s="24">
         <v>104166.66666666701</v>
       </c>
       <c r="F56">
@@ -1577,19 +1612,19 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="29">
         <v>4.6296296296296298</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="I57" s="16">
+      <c r="I57" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="J57" s="16">
+      <c r="J57" s="30">
         <v>-0.92592592592592604</v>
       </c>
     </row>
@@ -1609,19 +1644,19 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58" s="16">
+      <c r="F58" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="G58" s="16">
+      <c r="G58" s="29">
         <v>4.6296296296296298</v>
       </c>
-      <c r="H58" s="16">
+      <c r="H58" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="I58" s="16">
+      <c r="I58" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="J58" s="16">
+      <c r="J58" s="30">
         <v>-0.92592592592592604</v>
       </c>
     </row>
@@ -1641,19 +1676,19 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" s="16">
+      <c r="F59" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="G59" s="16">
+      <c r="G59" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="H59" s="16">
+      <c r="H59" s="29">
         <v>4.6296296296296298</v>
       </c>
-      <c r="I59" s="16">
+      <c r="I59" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="J59" s="16">
+      <c r="J59" s="30">
         <v>-0.92592592592592604</v>
       </c>
     </row>
@@ -1673,19 +1708,19 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60" s="16">
+      <c r="F60" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="G60" s="16">
+      <c r="G60" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="H60" s="16">
+      <c r="H60" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="I60" s="16">
+      <c r="I60" s="29">
         <v>4.6296296296296298</v>
       </c>
-      <c r="J60" s="16">
+      <c r="J60" s="30">
         <v>-0.92592592592592604</v>
       </c>
     </row>
@@ -1705,19 +1740,19 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F61" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="G61" s="16">
+      <c r="G61" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="I61" s="16">
+      <c r="I61" s="30">
         <v>-0.92592592592592604</v>
       </c>
-      <c r="J61" s="16">
+      <c r="J61" s="29">
         <v>4.6296296296296298</v>
       </c>
     </row>
@@ -1737,10 +1772,10 @@
       <c r="A66" s="16">
         <v>4</v>
       </c>
-      <c r="B66" s="16">
+      <c r="B66" s="23">
         <v>23408188.068984602</v>
       </c>
-      <c r="C66" s="16">
+      <c r="C66" s="23">
         <v>23408458.108272899</v>
       </c>
     </row>
@@ -1748,10 +1783,10 @@
       <c r="A67" s="16">
         <v>5</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="21">
         <v>21632913.6591</v>
       </c>
-      <c r="C67" s="16">
+      <c r="C67" s="23">
         <v>21633431.795521699</v>
       </c>
     </row>
@@ -1759,10 +1794,10 @@
       <c r="A68" s="16">
         <v>6</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="23">
         <v>21371250.344638199</v>
       </c>
-      <c r="C68" s="16">
+      <c r="C68" s="22">
         <v>21371107.054242</v>
       </c>
     </row>
@@ -1770,10 +1805,10 @@
       <c r="A69" s="16">
         <v>20</v>
       </c>
-      <c r="B69" s="16">
+      <c r="B69" s="23">
         <v>20127388.690065101</v>
       </c>
-      <c r="C69" s="16">
+      <c r="C69" s="23">
         <v>20127430.4542275</v>
       </c>
     </row>
@@ -1781,10 +1816,10 @@
       <c r="A70" s="16">
         <v>24</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="23">
         <v>21915054.787798598</v>
       </c>
-      <c r="C70" s="16">
+      <c r="C70" s="23">
         <v>21915515.096868198</v>
       </c>
     </row>
@@ -1792,18 +1827,18 @@
       <c r="A71" s="16">
         <v>25</v>
       </c>
-      <c r="B71" s="16">
+      <c r="B71" s="23">
         <v>21939371.838162899</v>
       </c>
-      <c r="C71" s="16">
+      <c r="C71" s="23">
         <v>21938803.045765299</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="21"/>
+      <c r="B76" s="20"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
@@ -1820,7 +1855,7 @@
       <c r="A78" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B78" s="16">
+      <c r="B78" s="25">
         <v>0.19029367280000001</v>
       </c>
       <c r="C78" t="s">

</xml_diff>